<commit_message>
Continuação projeto Fluxo de Caixa
</commit_message>
<xml_diff>
--- a/Modulo 14 [PROJETO] - Projeto Fluxo de caixa/projeto-fluxo-de-caixa-02.xlsx
+++ b/Modulo 14 [PROJETO] - Projeto Fluxo de caixa/projeto-fluxo-de-caixa-02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Curso-Excel\Modulo 14 [PROJETO] - Projeto Fluxo de caixa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2D466C-04B6-4E8F-90DA-9DE94C8AAFAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053AEFDD-6B24-4BA0-9986-7AB6B5BB1014}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
   </sheets>
   <definedNames>
     <definedName name="PCEntradasN1_Nível_1">TbPCEntradasN1[Nível 1]</definedName>
+    <definedName name="PCSaídasN1_Nível_1">TbPCSaídasN1[Nível 1]</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="61">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -182,6 +183,51 @@
   </si>
   <si>
     <t>Impostos sobre as vendas</t>
+  </si>
+  <si>
+    <t>Vestuário</t>
+  </si>
+  <si>
+    <t>Comunicação - internet e telefonia</t>
+  </si>
+  <si>
+    <t>Energia elétrica</t>
+  </si>
+  <si>
+    <t>Encargos sobre os salários dos vendedores</t>
+  </si>
+  <si>
+    <t>Salários dos vendedores</t>
+  </si>
+  <si>
+    <t>Juros sobre empréstimos</t>
+  </si>
+  <si>
+    <t>IR sobre o lucro presumido</t>
+  </si>
+  <si>
+    <t>PLANO DE CONTAS DE SAÍDAS NIVEL 2</t>
+  </si>
+  <si>
+    <t>Data do Caixa realizado</t>
+  </si>
+  <si>
+    <t>Data da competência</t>
+  </si>
+  <si>
+    <t>Data do Caixa previsto</t>
+  </si>
+  <si>
+    <t>Conta Nível 1</t>
+  </si>
+  <si>
+    <t>Conta Nível 2</t>
+  </si>
+  <si>
+    <t>Histórico</t>
+  </si>
+  <si>
+    <t>Valor</t>
   </si>
 </sst>
 </file>
@@ -315,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -328,9 +374,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -341,11 +384,25 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2991,7 +3048,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{446B8D0C-9026-4068-BA4F-3B4701745076}" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{446B8D0C-9026-4068-BA4F-3B4701745076}" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="B4:B9" xr:uid="{95D69D35-8ACD-4714-9657-4C387D2F5A69}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{33ECE0A5-989D-4CE3-A16B-DDA967DD4FB4}" name="Nível 1"/>
@@ -3001,7 +3058,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E42671F0-8465-4DA0-BF0B-7A93F9D0F44F}" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C12" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E42671F0-8465-4DA0-BF0B-7A93F9D0F44F}" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C12" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="B4:C12" xr:uid="{76A11DFF-3380-41A9-B4AF-7CA9211D129A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{27AB2540-2C04-4213-BD04-EDC1A3E67D90}" name="Nível 1"/>
@@ -3012,10 +3069,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3D8AB8E7-4D31-4C49-A326-1D7CB54DB1A3}" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3D8AB8E7-4D31-4C49-A326-1D7CB54DB1A3}" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="B4:B10" xr:uid="{3D9BB22D-17B7-487F-A4B5-1F64409EE153}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{72EBE09B-3C3D-4202-819D-0984BC93D865}" name="Nível 1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CDF5DF52-B992-4D63-AE7B-DE2C9B826280}" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C15" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B4:C15" xr:uid="{64625FE3-A89E-4904-A476-D233DF341444}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D9637226-85BB-4AF4-8579-9CBBEEBF3125}" name="Nível 1"/>
+    <tableColumn id="2" xr3:uid="{C7B5DC88-8047-439C-AFB8-3E331A30E10D}" name="Nível 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4011,7 +4079,7 @@
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="7"/>
@@ -4028,7 +4096,7 @@
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="7"/>
@@ -4143,10 +4211,10 @@
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -4160,10 +4228,10 @@
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="7"/>
@@ -4279,9 +4347,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B5:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4331,7 +4399,7 @@
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="7"/>
@@ -4348,7 +4416,7 @@
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="7"/>
@@ -4414,15 +4482,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.81640625" customWidth="1"/>
     <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="3" max="3" width="42.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
@@ -4462,24 +4531,146 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B15" xr:uid="{9CBD2ADA-04D7-4074-8894-370163EAE9E9}">
+      <formula1>PCSaídasN1_Nível_1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -4487,18 +4678,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
+    <col min="2" max="2" width="18.36328125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" customWidth="1"/>
+    <col min="6" max="6" width="21.08984375" customWidth="1"/>
+    <col min="7" max="7" width="19.1796875" customWidth="1"/>
+    <col min="8" max="8" width="24.90625" customWidth="1"/>
+    <col min="9" max="9" width="2.54296875" customWidth="1"/>
     <col min="16" max="16384" width="9.1796875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4510,17 +4708,11 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -4528,27 +4720,43 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    </row>
+    <row r="3" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4658,13 +4866,13 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>

</xml_diff>

<commit_message>
Validação conta Nivel 2 (RegistroEntradas)
</commit_message>
<xml_diff>
--- a/Modulo 14 [PROJETO] - Projeto Fluxo de caixa/projeto-fluxo-de-caixa-02.xlsx
+++ b/Modulo 14 [PROJETO] - Projeto Fluxo de caixa/projeto-fluxo-de-caixa-02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Curso-Excel\Modulo 14 [PROJETO] - Projeto Fluxo de caixa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053AEFDD-6B24-4BA0-9986-7AB6B5BB1014}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1202F9BC-781B-40F2-B888-7C65FA990A4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,6 +32,8 @@
   </sheets>
   <definedNames>
     <definedName name="PCEntradasN1_Nível_1">TbPCEntradasN1[Nível 1]</definedName>
+    <definedName name="PCEntradasN2_Nível_1">TbPCEntradasN2[Nível 1]</definedName>
+    <definedName name="PCEntradasN2_Nível_2">TbPCEntradasN2[Nível 2]</definedName>
     <definedName name="PCSaídasN1_Nível_1">TbPCSaídasN1[Nível 1]</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="65">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -228,12 +230,27 @@
   </si>
   <si>
     <t>Valor</t>
+  </si>
+  <si>
+    <t>NF773</t>
+  </si>
+  <si>
+    <t>NF2639</t>
+  </si>
+  <si>
+    <t>NF-16</t>
+  </si>
+  <si>
+    <t>Geral</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -361,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -387,14 +404,50 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3048,7 +3101,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{446B8D0C-9026-4068-BA4F-3B4701745076}" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{446B8D0C-9026-4068-BA4F-3B4701745076}" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="B4:B9" xr:uid="{95D69D35-8ACD-4714-9657-4C387D2F5A69}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{33ECE0A5-989D-4CE3-A16B-DDA967DD4FB4}" name="Nível 1"/>
@@ -3058,8 +3111,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E42671F0-8465-4DA0-BF0B-7A93F9D0F44F}" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C12" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="B4:C12" xr:uid="{76A11DFF-3380-41A9-B4AF-7CA9211D129A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E42671F0-8465-4DA0-BF0B-7A93F9D0F44F}" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C13" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="B4:C13" xr:uid="{76A11DFF-3380-41A9-B4AF-7CA9211D129A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{27AB2540-2C04-4213-BD04-EDC1A3E67D90}" name="Nível 1"/>
     <tableColumn id="2" xr3:uid="{1951752E-7577-4277-A945-1DAF76111BBE}" name="Nível 2"/>
@@ -3069,7 +3122,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3D8AB8E7-4D31-4C49-A326-1D7CB54DB1A3}" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3D8AB8E7-4D31-4C49-A326-1D7CB54DB1A3}" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="B4:B10" xr:uid="{3D9BB22D-17B7-487F-A4B5-1F64409EE153}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{72EBE09B-3C3D-4202-819D-0984BC93D865}" name="Nível 1"/>
@@ -3079,11 +3132,27 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CDF5DF52-B992-4D63-AE7B-DE2C9B826280}" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C15" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CDF5DF52-B992-4D63-AE7B-DE2C9B826280}" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C15" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="B4:C15" xr:uid="{64625FE3-A89E-4904-A476-D233DF341444}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D9637226-85BB-4AF4-8579-9CBBEEBF3125}" name="Nível 1"/>
     <tableColumn id="2" xr3:uid="{C7B5DC88-8047-439C-AFB8-3E331A30E10D}" name="Nível 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0F593BC3-37E0-4D73-B3C4-B3BFDA5F2CE0}" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B3:H7" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B3:H7" xr:uid="{E19EEC21-6327-4635-A5D4-949353ABE634}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{CF820E5C-6DA6-4707-951B-B39BBC8F6BC3}" name="Data do Caixa realizado" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{EE4F1D68-6863-40B2-A41F-FCBA698B83FD}" name="Data da competência" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{6A4C8C78-BFA0-499A-80C0-7DD6164E6611}" name="Data do Caixa previsto" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{B1A08430-A222-42BA-9634-EBBB002735C3}" name="Conta Nível 1"/>
+    <tableColumn id="5" xr3:uid="{65C22766-AE40-4081-9AAC-81D91EA88C9F}" name="Conta Nível 2"/>
+    <tableColumn id="6" xr3:uid="{F8623FC7-98A7-4ECB-A84E-62F7C9B97901}" name="Histórico"/>
+    <tableColumn id="7" xr3:uid="{2491F392-CECB-48D1-92A4-3D0DE28D14FE}" name="Valor" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4159,8 +4228,8 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4321,7 +4390,14 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4331,7 +4407,7 @@
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B12" xr:uid="{CC017BE4-5880-421F-89D2-EC78E8F7C853}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B13" xr:uid="{CC017BE4-5880-421F-89D2-EC78E8F7C853}">
       <formula1>PCEntradasN1_Nível_1</formula1>
     </dataValidation>
   </dataValidations>
@@ -4480,7 +4556,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -4679,20 +4755,22 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.36328125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" customWidth="1"/>
-    <col min="6" max="6" width="21.08984375" customWidth="1"/>
-    <col min="7" max="7" width="19.1796875" customWidth="1"/>
-    <col min="8" max="8" width="24.90625" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" customWidth="1"/>
+    <col min="6" max="6" width="29.81640625" customWidth="1"/>
+    <col min="7" max="7" width="21.26953125" customWidth="1"/>
+    <col min="8" max="8" width="24.90625" style="16" customWidth="1"/>
     <col min="9" max="9" width="2.54296875" customWidth="1"/>
+    <col min="10" max="15" width="0" hidden="1" customWidth="1"/>
     <col min="16" max="16384" width="9.1796875" hidden="1"/>
   </cols>
   <sheetData>
@@ -4708,7 +4786,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4719,35 +4797,123 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="13" t="s">
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="13">
+        <v>43146</v>
+      </c>
+      <c r="C4" s="13">
+        <v>43146</v>
+      </c>
+      <c r="D4" s="13">
+        <v>43146</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="13">
+        <v>43530</v>
+      </c>
+      <c r="C5" s="13">
+        <v>43466</v>
+      </c>
+      <c r="D5" s="13">
+        <v>43496</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="16">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="13">
+        <v>43467</v>
+      </c>
+      <c r="C6" s="13">
+        <v>43467</v>
+      </c>
+      <c r="D6" s="13">
+        <v>43467</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="16">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="13">
+        <v>43535</v>
+      </c>
+      <c r="C7" s="13">
+        <v>43467</v>
+      </c>
+      <c r="D7" s="13">
+        <v>43497</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="16">
+        <v>34</v>
+      </c>
+    </row>
     <row r="8" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4759,8 +4925,19 @@
     <row r="16" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E7" xr:uid="{895437C2-CF83-4925-BFA8-1E10791076C5}">
+      <formula1 xml:space="preserve"> PCEntradasN1_Nível_1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F7" xr:uid="{C9EECD50-3520-47D0-B73A-C2832948788E}">
+      <formula1>OFFSET(PCEntradasN2_Nível_2,MATCH(E4,PCEntradasN2_Nível_1,0)-1,0,COUNTIF(PCEntradasN2_Nível_1,E4))</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Finalizando aula 13 e organizando aulas
</commit_message>
<xml_diff>
--- a/Modulo 14 [PROJETO] - Projeto Fluxo de caixa/projeto-fluxo-de-caixa-02.xlsx
+++ b/Modulo 14 [PROJETO] - Projeto Fluxo de caixa/projeto-fluxo-de-caixa-02.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Curso-Excel\Modulo 14 [PROJETO] - Projeto Fluxo de caixa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelio\Documents\Curso Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1202F9BC-781B-40F2-B888-7C65FA990A4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -30,12 +29,6 @@
     <sheet name="DashBoardFinanceiroAtual" sheetId="15" r:id="rId15"/>
     <sheet name="DashBoardFinanceiroMensal" sheetId="16" r:id="rId16"/>
   </sheets>
-  <definedNames>
-    <definedName name="PCEntradasN1_Nível_1">TbPCEntradasN1[Nível 1]</definedName>
-    <definedName name="PCEntradasN2_Nível_1">TbPCEntradasN2[Nível 1]</definedName>
-    <definedName name="PCEntradasN2_Nível_2">TbPCEntradasN2[Nível 2]</definedName>
-    <definedName name="PCSaídasN1_Nível_1">TbPCSaídasN1[Nível 1]</definedName>
-  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -114,144 +107,12 @@
   <si>
     <t>DASHBOARD FINANCEIRO - POSIÇÃO MENSAL</t>
   </si>
-  <si>
-    <t>PLANO DE CONTAS DE ENTRADAS NÍVEL 1</t>
-  </si>
-  <si>
-    <t>Nível 1</t>
-  </si>
-  <si>
-    <t>Empréstimos de curto prazo</t>
-  </si>
-  <si>
-    <t>Financiamentos de longo prazo</t>
-  </si>
-  <si>
-    <t>Receitas Financeiras</t>
-  </si>
-  <si>
-    <t>Venda de ativos</t>
-  </si>
-  <si>
-    <t>Vendas de mercadorias</t>
-  </si>
-  <si>
-    <t>PLANO DE CONTAS DE ENTRADAS NÍVEL 2</t>
-  </si>
-  <si>
-    <t>Nível 2</t>
-  </si>
-  <si>
-    <t>Empréstimos capital de giro</t>
-  </si>
-  <si>
-    <t>Juros sobre aplicações</t>
-  </si>
-  <si>
-    <t>Mobiliário próprio</t>
-  </si>
-  <si>
-    <t>Eletrodomésticos</t>
-  </si>
-  <si>
-    <t>Informática</t>
-  </si>
-  <si>
-    <t>Livros</t>
-  </si>
-  <si>
-    <t>Móveis</t>
-  </si>
-  <si>
-    <t>Som e imagem</t>
-  </si>
-  <si>
-    <t>PLANO DE CONTAS DE SAÍDA NÍVEL 1</t>
-  </si>
-  <si>
-    <t>Compra de mercadorias</t>
-  </si>
-  <si>
-    <t>Despesas administrativas</t>
-  </si>
-  <si>
-    <t>Despesas comerciais</t>
-  </si>
-  <si>
-    <t>Despesas financeiras</t>
-  </si>
-  <si>
-    <t>Imposto de renda</t>
-  </si>
-  <si>
-    <t>Impostos sobre as vendas</t>
-  </si>
-  <si>
-    <t>Vestuário</t>
-  </si>
-  <si>
-    <t>Comunicação - internet e telefonia</t>
-  </si>
-  <si>
-    <t>Energia elétrica</t>
-  </si>
-  <si>
-    <t>Encargos sobre os salários dos vendedores</t>
-  </si>
-  <si>
-    <t>Salários dos vendedores</t>
-  </si>
-  <si>
-    <t>Juros sobre empréstimos</t>
-  </si>
-  <si>
-    <t>IR sobre o lucro presumido</t>
-  </si>
-  <si>
-    <t>PLANO DE CONTAS DE SAÍDAS NIVEL 2</t>
-  </si>
-  <si>
-    <t>Data do Caixa realizado</t>
-  </si>
-  <si>
-    <t>Data da competência</t>
-  </si>
-  <si>
-    <t>Data do Caixa previsto</t>
-  </si>
-  <si>
-    <t>Conta Nível 1</t>
-  </si>
-  <si>
-    <t>Conta Nível 2</t>
-  </si>
-  <si>
-    <t>Histórico</t>
-  </si>
-  <si>
-    <t>Valor</t>
-  </si>
-  <si>
-    <t>NF773</t>
-  </si>
-  <si>
-    <t>NF2639</t>
-  </si>
-  <si>
-    <t>NF-16</t>
-  </si>
-  <si>
-    <t>Geral</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,14 +151,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -325,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -333,52 +186,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.24994659260841701"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.24994659260841701"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="2" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="2" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -391,96 +203,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -510,13 +240,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Retângulo 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Retângulo 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -588,13 +312,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Retângulo 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="8" name="Retângulo 7"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -666,13 +384,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Retângulo 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="9" name="Retângulo 8"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -746,11 +458,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="Retângulo 9">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -835,11 +542,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="11" name="Retângulo 10">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -911,11 +613,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="12" name="Retângulo 11">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -987,11 +684,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="13" name="Retângulo 12">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -1063,11 +755,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="14" name="Retângulo 13">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -1152,11 +839,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="15" name="Retângulo 14">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -1228,11 +910,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="16" name="Retângulo 15">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -1304,11 +981,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="17" name="Retângulo 16">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -1380,11 +1052,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="18" name="Retângulo 17">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -1456,11 +1123,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="19" name="Retângulo 18">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -1532,11 +1194,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="20" name="Retângulo 19">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -1608,11 +1265,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="21" name="Retângulo 20">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -1697,11 +1349,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="22" name="Retângulo 21">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -1773,11 +1420,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="23" name="Retângulo 22">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -1847,13 +1489,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Imagem 27">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="28" name="Imagem 27"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1904,11 +1540,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -1985,11 +1616,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -2066,11 +1692,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -2147,11 +1768,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -2228,11 +1844,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -2309,11 +1920,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -2390,11 +1996,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -2471,11 +2072,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="20" name="Retângulo 19">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -2552,11 +2148,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -2633,11 +2224,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -2714,11 +2300,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -2795,11 +2376,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -2876,11 +2452,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -2957,11 +2528,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -3038,11 +2604,6 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
-            </a:ext>
-          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -3098,64 +2659,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{446B8D0C-9026-4068-BA4F-3B4701745076}" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="B4:B9" xr:uid="{95D69D35-8ACD-4714-9657-4C387D2F5A69}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{33ECE0A5-989D-4CE3-A16B-DDA967DD4FB4}" name="Nível 1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E42671F0-8465-4DA0-BF0B-7A93F9D0F44F}" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C13" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="B4:C13" xr:uid="{76A11DFF-3380-41A9-B4AF-7CA9211D129A}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{27AB2540-2C04-4213-BD04-EDC1A3E67D90}" name="Nível 1"/>
-    <tableColumn id="2" xr3:uid="{1951752E-7577-4277-A945-1DAF76111BBE}" name="Nível 2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3D8AB8E7-4D31-4C49-A326-1D7CB54DB1A3}" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="B4:B10" xr:uid="{3D9BB22D-17B7-487F-A4B5-1F64409EE153}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{72EBE09B-3C3D-4202-819D-0984BC93D865}" name="Nível 1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CDF5DF52-B992-4D63-AE7B-DE2C9B826280}" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C15" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="B4:C15" xr:uid="{64625FE3-A89E-4904-A476-D233DF341444}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D9637226-85BB-4AF4-8579-9CBBEEBF3125}" name="Nível 1"/>
-    <tableColumn id="2" xr3:uid="{C7B5DC88-8047-439C-AFB8-3E331A30E10D}" name="Nível 2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0F593BC3-37E0-4D73-B3C4-B3BFDA5F2CE0}" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B3:H7" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B3:H7" xr:uid="{E19EEC21-6327-4635-A5D4-949353ABE634}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CF820E5C-6DA6-4707-951B-B39BBC8F6BC3}" name="Data do Caixa realizado" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{EE4F1D68-6863-40B2-A41F-FCBA698B83FD}" name="Data da competência" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{6A4C8C78-BFA0-499A-80C0-7DD6164E6611}" name="Data do Caixa previsto" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{B1A08430-A222-42BA-9634-EBBB002735C3}" name="Conta Nível 1"/>
-    <tableColumn id="5" xr3:uid="{65C22766-AE40-4081-9AAC-81D91EA88C9F}" name="Conta Nível 2"/>
-    <tableColumn id="6" xr3:uid="{F8623FC7-98A7-4ECB-A84E-62F7C9B97901}" name="Histórico"/>
-    <tableColumn id="7" xr3:uid="{2491F392-CECB-48D1-92A4-3D0DE28D14FE}" name="Valor" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3420,21 +2923,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3456,37 +2959,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -3499,7 +3002,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -3507,21 +3010,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3543,7 +3046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -3558,21 +3061,21 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -3580,21 +3083,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3616,7 +3119,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -3631,21 +3134,21 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -3653,21 +3156,21 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3689,7 +3192,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -3704,21 +3207,21 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -3726,21 +3229,21 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3762,7 +3265,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -3777,21 +3280,21 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -3799,21 +3302,21 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3835,7 +3338,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -3850,21 +3353,21 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -3872,21 +3375,21 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3908,7 +3411,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -3923,21 +3426,21 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -3945,21 +3448,21 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3981,7 +3484,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -3996,21 +3499,21 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -4018,23 +3521,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4056,7 +3559,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -4071,21 +3574,21 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -4093,24 +3596,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B9"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4132,7 +3632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -4147,102 +3647,43 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-    </row>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="3" width="28.90625" customWidth="1"/>
-    <col min="4" max="14" width="8.6328125" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4264,7 +3705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -4279,165 +3720,43 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-    </row>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-    </row>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:C3"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B13" xr:uid="{CC017BE4-5880-421F-89D2-EC78E8F7C853}">
-      <formula1>PCEntradasN1_Nível_1</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B5:B10"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4459,7 +3778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -4474,103 +3793,43 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-    </row>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="3" width="42.90625" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4592,7 +3851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -4607,356 +3866,43 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-    </row>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:C3"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B15" xr:uid="{9CBD2ADA-04D7-4074-8894-370163EAE9E9}">
-      <formula1>PCSaídasN1_Nível_1</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:O17"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" customWidth="1"/>
-    <col min="6" max="6" width="29.81640625" customWidth="1"/>
-    <col min="7" max="7" width="21.26953125" customWidth="1"/>
-    <col min="8" max="8" width="24.90625" style="16" customWidth="1"/>
-    <col min="9" max="9" width="2.54296875" customWidth="1"/>
-    <col min="10" max="15" width="0" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="1:8" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="13">
-        <v>43146</v>
-      </c>
-      <c r="C4" s="13">
-        <v>43146</v>
-      </c>
-      <c r="D4" s="13">
-        <v>43146</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="16">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="13">
-        <v>43530</v>
-      </c>
-      <c r="C5" s="13">
-        <v>43466</v>
-      </c>
-      <c r="D5" s="13">
-        <v>43496</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="16">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="13">
-        <v>43467</v>
-      </c>
-      <c r="C6" s="13">
-        <v>43467</v>
-      </c>
-      <c r="D6" s="13">
-        <v>43467</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="16">
-        <v>2689</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="13">
-        <v>43535</v>
-      </c>
-      <c r="C7" s="13">
-        <v>43467</v>
-      </c>
-      <c r="D7" s="13">
-        <v>43497</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="16">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E7" xr:uid="{895437C2-CF83-4925-BFA8-1E10791076C5}">
-      <formula1 xml:space="preserve"> PCEntradasN1_Nível_1</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F7" xr:uid="{C9EECD50-3520-47D0-B73A-C2832948788E}">
-      <formula1>OFFSET(PCEntradasN2_Nível_2,MATCH(E4,PCEntradasN2_Nível_1,0)-1,0,COUNTIF(PCEntradasN2_Nível_1,E4))</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4975,10 +3921,10 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -4993,43 +3939,43 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="2.54296875" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" hidden="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -5043,15 +3989,15 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -5066,21 +4012,94 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J1:N1"/>

</xml_diff>